<commit_message>
KARMEN DPE and DD (Tracy and Ines)
</commit_message>
<xml_diff>
--- a/Ines/DD_KARMEN_INES.xlsx
+++ b/Ines/DD_KARMEN_INES.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Ines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\Ines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCCDCE-896B-4A88-807A-CA02AB48C502}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12230"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>index</t>
   </si>
@@ -41,13 +40,160 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>KL_TG</t>
+  </si>
+  <si>
+    <t>Triglycerides</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>KL_CHO</t>
+  </si>
+  <si>
+    <t>Total Cholesterol</t>
+  </si>
+  <si>
+    <t>KL_LDLC</t>
+  </si>
+  <si>
+    <t>LDL-Cholesterol</t>
+  </si>
+  <si>
+    <t>KL_HDLC</t>
+  </si>
+  <si>
+    <t>HDL-Cholesterol</t>
+  </si>
+  <si>
+    <t>kcal_zb_tag_NCI</t>
+  </si>
+  <si>
+    <t>Energy intake [kcal/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kh_tag_NCI </t>
+  </si>
+  <si>
+    <t>Carbohydrate intake [g/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prot_tag_NCI  </t>
+  </si>
+  <si>
+    <t>Protein intake [g/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_tag_NCI </t>
+  </si>
+  <si>
+    <t>Fat intake [g/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">al_tag_NCI </t>
+  </si>
+  <si>
+    <t>Alcohol intake [g/d]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bs_tag_NCI </t>
+  </si>
+  <si>
+    <t>Dietary fiber intake [g/d]</t>
+  </si>
+  <si>
+    <t>fsges_tag_NCI</t>
+  </si>
+  <si>
+    <t>Saturated fat intake [g/d]</t>
+  </si>
+  <si>
+    <t>fseuges_tag_NCI</t>
+  </si>
+  <si>
+    <t>Monounsaturated fat intake [g/d]</t>
+  </si>
+  <si>
+    <t>fsmuges_tag_NCI</t>
+  </si>
+  <si>
+    <t>Polyunsaturated fat intake [g/d]</t>
+  </si>
+  <si>
+    <t>KMD_tag</t>
+  </si>
+  <si>
+    <t>Total sugar intake [g/d]</t>
+  </si>
+  <si>
+    <t>KMT_tag</t>
+  </si>
+  <si>
+    <t>Glucose intake [g/d]</t>
+  </si>
+  <si>
+    <t>KMF_tag</t>
+  </si>
+  <si>
+    <t>Fructose intake [g/d]</t>
+  </si>
+  <si>
+    <t>na_tag_NCI</t>
+  </si>
+  <si>
+    <t>Sodium intake [g/d]</t>
+  </si>
+  <si>
+    <t>k_tag_NCI</t>
+  </si>
+  <si>
+    <t>Potassium intake [g/d]</t>
+  </si>
+  <si>
+    <t>Alter_BE</t>
+  </si>
+  <si>
+    <t>Age at blood sampling</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>Body Mass Index (BMI)</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>waist circumference</t>
+  </si>
+  <si>
+    <t>FR_android</t>
+  </si>
+  <si>
+    <t>%body fat - Android region (related to total body mass as assessed by DXA)</t>
+  </si>
+  <si>
+    <t>FR_gynoid</t>
+  </si>
+  <si>
+    <t>%body fat - Gynoid region (related to total body mass as assessed by DXA)</t>
+  </si>
+  <si>
+    <t>FMI</t>
+  </si>
+  <si>
+    <t>Fat Mass Index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +205,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -84,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -101,9 +261,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,22 +594,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="3"/>
-    <col min="2" max="2" width="26.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="157.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="5"/>
+    <col min="1" max="1" width="11.453125" style="3"/>
+    <col min="2" max="2" width="26.26953125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="157.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,559 +623,690 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="11"/>
+      <c r="B7" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="11"/>
+      <c r="B8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="11"/>
+      <c r="B9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
+      <c r="B20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
+      <c r="B21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>33</v>
+      </c>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
+      <c r="B23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="D23"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
+      <c r="B24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="D24"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
+      <c r="B25" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="D25"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -1008,21 +1319,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="30.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="3"/>
+    <col min="3" max="3" width="30.54296875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1040,15 +1351,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
@@ -1060,7 +1362,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -1301,15 +1603,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1326,7 +1629,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{607F74A7-32EE-406C-A688-0D84C4E12BE8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1343,4 +1646,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>